<commit_message>
Appended/Updated sheet 'HOTCARD' via Github_Excel_Append_Tool
</commit_message>
<xml_diff>
--- a/Hotcard Wave Spreadsheet.xlsx
+++ b/Hotcard Wave Spreadsheet.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:CT3"/>
+  <dimension ref="A1:DC4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -922,6 +922,51 @@
       <c r="CT1" s="1" t="inlineStr">
         <is>
           <t>CREQ#</t>
+        </is>
+      </c>
+      <c r="CU1" s="1" t="inlineStr">
+        <is>
+          <t>Migration Date</t>
+        </is>
+      </c>
+      <c r="CV1" s="1" t="inlineStr">
+        <is>
+          <t>FI Name</t>
+        </is>
+      </c>
+      <c r="CW1" s="1" t="inlineStr">
+        <is>
+          <t>Switch: FISB</t>
+        </is>
+      </c>
+      <c r="CX1" s="1" t="inlineStr">
+        <is>
+          <t>Old Platform</t>
+        </is>
+      </c>
+      <c r="CY1" s="1" t="inlineStr">
+        <is>
+          <t>New Platform :PaymentsOne Debit</t>
+        </is>
+      </c>
+      <c r="CZ1" s="1" t="inlineStr">
+        <is>
+          <t>Service: Basic</t>
+        </is>
+      </c>
+      <c r="DA1" s="1" t="inlineStr">
+        <is>
+          <t>CS Location: Offshore</t>
+        </is>
+      </c>
+      <c r="DB1" s="1" t="inlineStr">
+        <is>
+          <t>Total Card Count</t>
+        </is>
+      </c>
+      <c r="DC1" s="1" t="inlineStr">
+        <is>
+          <t>Using OneCall IVR</t>
         </is>
       </c>
     </row>
@@ -971,10 +1016,8 @@
           <t>IL</t>
         </is>
       </c>
-      <c r="R2" t="inlineStr">
-        <is>
-          <t>62701</t>
-        </is>
+      <c r="R2" t="n">
+        <v>62701</v>
       </c>
       <c r="S2" t="inlineStr">
         <is>
@@ -1083,10 +1126,8 @@
           <t>Entrust</t>
         </is>
       </c>
-      <c r="AP2" t="inlineStr">
-        <is>
-          <t>123456789</t>
-        </is>
+      <c r="AP2" t="n">
+        <v>123456789</v>
       </c>
       <c r="AQ2" t="inlineStr"/>
       <c r="AR2" t="inlineStr">
@@ -1116,15 +1157,11 @@
       </c>
       <c r="AW2" t="inlineStr"/>
       <c r="AX2" t="inlineStr"/>
-      <c r="AY2" t="inlineStr">
-        <is>
-          <t>123456</t>
-        </is>
-      </c>
-      <c r="AZ2" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
+      <c r="AY2" t="n">
+        <v>123456</v>
+      </c>
+      <c r="AZ2" t="n">
+        <v>6</v>
       </c>
       <c r="BA2" t="inlineStr">
         <is>
@@ -1197,10 +1234,8 @@
           <t>192.168.1.1</t>
         </is>
       </c>
-      <c r="BP2" t="inlineStr">
-        <is>
-          <t>8080</t>
-        </is>
+      <c r="BP2" t="n">
+        <v>8080</v>
       </c>
       <c r="BQ2" t="inlineStr">
         <is>
@@ -1337,10 +1372,8 @@
           <t>Debit, Credit</t>
         </is>
       </c>
-      <c r="CR2" t="inlineStr">
-        <is>
-          <t>15000</t>
-        </is>
+      <c r="CR2" t="n">
+        <v>15000</v>
       </c>
       <c r="CS2" t="inlineStr">
         <is>
@@ -1352,6 +1385,15 @@
           <t>CREQ789</t>
         </is>
       </c>
+      <c r="CU2" t="inlineStr"/>
+      <c r="CV2" t="inlineStr"/>
+      <c r="CW2" t="inlineStr"/>
+      <c r="CX2" t="inlineStr"/>
+      <c r="CY2" t="inlineStr"/>
+      <c r="CZ2" t="inlineStr"/>
+      <c r="DA2" t="inlineStr"/>
+      <c r="DB2" t="inlineStr"/>
+      <c r="DC2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr"/>
@@ -1399,10 +1441,8 @@
           <t>IL</t>
         </is>
       </c>
-      <c r="R3" t="inlineStr">
-        <is>
-          <t>62701</t>
-        </is>
+      <c r="R3" t="n">
+        <v>62701</v>
       </c>
       <c r="S3" t="inlineStr">
         <is>
@@ -1511,10 +1551,8 @@
           <t>Entrust</t>
         </is>
       </c>
-      <c r="AP3" t="inlineStr">
-        <is>
-          <t>123456789</t>
-        </is>
+      <c r="AP3" t="n">
+        <v>123456789</v>
       </c>
       <c r="AQ3" t="inlineStr"/>
       <c r="AR3" t="inlineStr">
@@ -1544,15 +1582,11 @@
       </c>
       <c r="AW3" t="inlineStr"/>
       <c r="AX3" t="inlineStr"/>
-      <c r="AY3" t="inlineStr">
-        <is>
-          <t>123456</t>
-        </is>
-      </c>
-      <c r="AZ3" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
+      <c r="AY3" t="n">
+        <v>123456</v>
+      </c>
+      <c r="AZ3" t="n">
+        <v>6</v>
       </c>
       <c r="BA3" t="inlineStr">
         <is>
@@ -1625,10 +1659,8 @@
           <t>192.168.1.1</t>
         </is>
       </c>
-      <c r="BP3" t="inlineStr">
-        <is>
-          <t>8080</t>
-        </is>
+      <c r="BP3" t="n">
+        <v>8080</v>
       </c>
       <c r="BQ3" t="inlineStr">
         <is>
@@ -1765,10 +1797,8 @@
           <t>Debit, Credit</t>
         </is>
       </c>
-      <c r="CR3" t="inlineStr">
-        <is>
-          <t>15000</t>
-        </is>
+      <c r="CR3" t="n">
+        <v>15000</v>
       </c>
       <c r="CS3" t="inlineStr">
         <is>
@@ -1778,6 +1808,164 @@
       <c r="CT3" t="inlineStr">
         <is>
           <t>CREQ789</t>
+        </is>
+      </c>
+      <c r="CU3" t="inlineStr"/>
+      <c r="CV3" t="inlineStr"/>
+      <c r="CW3" t="inlineStr"/>
+      <c r="CX3" t="inlineStr"/>
+      <c r="CY3" t="inlineStr"/>
+      <c r="CZ3" t="inlineStr"/>
+      <c r="DA3" t="inlineStr"/>
+      <c r="DB3" t="inlineStr"/>
+      <c r="DC3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr"/>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>123abx007</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
+      <c r="P4" t="inlineStr"/>
+      <c r="Q4" t="inlineStr"/>
+      <c r="R4" t="inlineStr"/>
+      <c r="S4" t="inlineStr"/>
+      <c r="T4" t="inlineStr"/>
+      <c r="U4" t="inlineStr"/>
+      <c r="V4" t="inlineStr"/>
+      <c r="W4" t="inlineStr"/>
+      <c r="X4" t="inlineStr"/>
+      <c r="Y4" t="inlineStr"/>
+      <c r="Z4" t="inlineStr"/>
+      <c r="AA4" t="inlineStr"/>
+      <c r="AB4" t="inlineStr"/>
+      <c r="AC4" t="inlineStr"/>
+      <c r="AD4" t="inlineStr"/>
+      <c r="AE4" t="inlineStr"/>
+      <c r="AF4" t="inlineStr"/>
+      <c r="AG4" t="inlineStr"/>
+      <c r="AH4" t="inlineStr"/>
+      <c r="AI4" t="inlineStr"/>
+      <c r="AJ4" t="inlineStr"/>
+      <c r="AK4" t="inlineStr"/>
+      <c r="AL4" t="inlineStr"/>
+      <c r="AM4" t="inlineStr"/>
+      <c r="AN4" t="inlineStr"/>
+      <c r="AO4" t="inlineStr"/>
+      <c r="AP4" t="inlineStr"/>
+      <c r="AQ4" t="inlineStr"/>
+      <c r="AR4" t="inlineStr"/>
+      <c r="AS4" t="inlineStr"/>
+      <c r="AT4" t="inlineStr"/>
+      <c r="AU4" t="inlineStr"/>
+      <c r="AV4" t="inlineStr"/>
+      <c r="AW4" t="inlineStr"/>
+      <c r="AX4" t="inlineStr"/>
+      <c r="AY4" t="inlineStr"/>
+      <c r="AZ4" t="inlineStr"/>
+      <c r="BA4" t="inlineStr"/>
+      <c r="BB4" t="inlineStr"/>
+      <c r="BC4" t="inlineStr"/>
+      <c r="BD4" t="inlineStr"/>
+      <c r="BE4" t="inlineStr"/>
+      <c r="BF4" t="inlineStr"/>
+      <c r="BG4" t="inlineStr"/>
+      <c r="BH4" t="inlineStr"/>
+      <c r="BI4" t="inlineStr"/>
+      <c r="BJ4" t="inlineStr"/>
+      <c r="BK4" t="inlineStr"/>
+      <c r="BL4" t="inlineStr"/>
+      <c r="BM4" t="inlineStr"/>
+      <c r="BN4" t="inlineStr"/>
+      <c r="BO4" t="inlineStr"/>
+      <c r="BP4" t="inlineStr"/>
+      <c r="BQ4" t="inlineStr"/>
+      <c r="BR4" t="inlineStr"/>
+      <c r="BS4" t="inlineStr"/>
+      <c r="BT4" t="inlineStr"/>
+      <c r="BU4" t="inlineStr"/>
+      <c r="BV4" t="inlineStr"/>
+      <c r="BW4" t="inlineStr"/>
+      <c r="BX4" t="inlineStr"/>
+      <c r="BY4" t="inlineStr"/>
+      <c r="BZ4" t="inlineStr"/>
+      <c r="CA4" t="inlineStr"/>
+      <c r="CB4" t="inlineStr"/>
+      <c r="CC4" t="inlineStr"/>
+      <c r="CD4" t="inlineStr"/>
+      <c r="CE4" t="inlineStr"/>
+      <c r="CF4" t="inlineStr"/>
+      <c r="CG4" t="inlineStr"/>
+      <c r="CH4" t="inlineStr"/>
+      <c r="CI4" t="inlineStr"/>
+      <c r="CJ4" t="inlineStr"/>
+      <c r="CK4" t="inlineStr"/>
+      <c r="CL4" t="inlineStr"/>
+      <c r="CM4" t="inlineStr"/>
+      <c r="CN4" t="inlineStr"/>
+      <c r="CO4" t="inlineStr"/>
+      <c r="CP4" t="inlineStr"/>
+      <c r="CQ4" t="inlineStr"/>
+      <c r="CR4" t="inlineStr"/>
+      <c r="CS4" t="inlineStr"/>
+      <c r="CT4" t="inlineStr"/>
+      <c r="CU4" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="CV4" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="CW4" t="inlineStr">
+        <is>
+          <t>FISB</t>
+        </is>
+      </c>
+      <c r="CX4" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="CY4" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="CZ4" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="DA4" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="DB4" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="DC4" t="inlineStr">
+        <is>
+          <t>NA</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated Excel while preserving formatting
</commit_message>
<xml_diff>
--- a/Hotcard Wave Spreadsheet.xlsx
+++ b/Hotcard Wave Spreadsheet.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U3"/>
+  <dimension ref="A1:U4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -541,16 +541,6 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr"/>
-      <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr">
         <is>
           <t>none</t>
@@ -608,16 +598,6 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr"/>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr">
         <is>
           <t>none</t>
@@ -671,6 +651,18 @@
       <c r="U3" t="inlineStr">
         <is>
           <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>2025-10-26</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>999FFF999</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated Migration Wave to 10/22/2001
</commit_message>
<xml_diff>
--- a/Hotcard Wave Spreadsheet.xlsx
+++ b/Hotcard Wave Spreadsheet.xlsx
@@ -1,103 +1,60 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vivek.lade\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE3F18E5-BB40-4720-947C-ECD6DA41EFB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="HOTCARD" sheetId="1" r:id="rId1"/>
+    <sheet name="HOTCARD" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
-  <si>
-    <t>Hotcarding Spreadsheet - Migration Wave 10/22/2001</t>
-  </si>
-  <si>
-    <t>Migration Date</t>
-  </si>
-  <si>
-    <t>FI Name</t>
-  </si>
-  <si>
-    <t>Entity ID</t>
-  </si>
-  <si>
-    <t>Switch</t>
-  </si>
-  <si>
-    <t>Old Platform</t>
-  </si>
-  <si>
-    <t>New Platform</t>
-  </si>
-  <si>
-    <t>Service</t>
-  </si>
-  <si>
-    <t>CS Location</t>
-  </si>
-  <si>
-    <t>Total Card Count</t>
-  </si>
-  <si>
-    <t>Using OneCall IVR</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="5">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Aptos"/>
       <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Aptos"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
     </font>
     <font>
-      <b/>
-      <sz val="14"/>
-      <color theme="0"/>
       <name val="Aptos"/>
       <family val="2"/>
+      <b val="1"/>
+      <color theme="0"/>
+      <sz val="14"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Aptos"/>
       <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="12"/>
     </font>
   </fonts>
   <fills count="4">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -110,7 +67,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <fgColor theme="0" tint="-0.0499893185216834"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -176,40 +133,99 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="12">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -509,106 +525,171 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:U4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="18.26953125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="30.453125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="21.26953125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.54296875" style="11" customWidth="1"/>
-    <col min="5" max="5" width="32.1796875" style="11" customWidth="1"/>
-    <col min="6" max="8" width="28.1796875" style="11" customWidth="1"/>
-    <col min="9" max="9" width="25.81640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="27.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.1796875" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.1796875" style="1"/>
+    <col width="18.26953125" customWidth="1" style="1" min="1" max="1"/>
+    <col width="30.453125" customWidth="1" style="1" min="2" max="2"/>
+    <col width="21.26953125" customWidth="1" style="1" min="3" max="3"/>
+    <col width="16.54296875" customWidth="1" style="11" min="4" max="4"/>
+    <col width="32.1796875" customWidth="1" style="11" min="5" max="5"/>
+    <col width="28.1796875" customWidth="1" style="11" min="6" max="8"/>
+    <col width="25.81640625" customWidth="1" style="1" min="9" max="9"/>
+    <col width="27.1796875" bestFit="1" customWidth="1" style="1" min="10" max="10"/>
+    <col width="9.1796875" customWidth="1" style="1" min="11" max="11"/>
+    <col width="9.1796875" customWidth="1" style="1" min="12" max="16384"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="5"/>
+    <row r="1" ht="30" customFormat="1" customHeight="1" s="2" thickBot="1">
+      <c r="A1" s="3" t="inlineStr">
+        <is>
+          <t>Hotcarding Spreadsheet - Migration Wave 10/22/2001</t>
+        </is>
+      </c>
+      <c r="B1" s="4" t="n"/>
+      <c r="C1" s="4" t="n"/>
+      <c r="D1" s="9" t="n"/>
+      <c r="E1" s="9" t="n"/>
+      <c r="F1" s="9" t="n"/>
+      <c r="G1" s="9" t="n"/>
+      <c r="H1" s="9" t="n"/>
+      <c r="I1" s="4" t="n"/>
+      <c r="J1" s="4" t="n"/>
+      <c r="K1" s="4" t="n"/>
+      <c r="L1" s="4" t="n"/>
+      <c r="M1" s="4" t="n"/>
+      <c r="N1" s="4" t="n"/>
+      <c r="O1" s="4" t="n"/>
+      <c r="P1" s="4" t="n"/>
+      <c r="Q1" s="4" t="n"/>
+      <c r="R1" s="4" t="n"/>
+      <c r="S1" s="4" t="n"/>
+      <c r="T1" s="4" t="n"/>
+      <c r="U1" s="5" t="n"/>
     </row>
-    <row r="2" spans="1:21" s="6" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
-      <c r="P2" s="7"/>
-      <c r="Q2" s="7"/>
-      <c r="R2" s="7"/>
-      <c r="S2" s="7"/>
-      <c r="T2" s="7"/>
-      <c r="U2" s="7"/>
+    <row r="2" ht="16" customFormat="1" customHeight="1" s="6">
+      <c r="A2" s="7" t="inlineStr">
+        <is>
+          <t>Migration Date</t>
+        </is>
+      </c>
+      <c r="B2" s="7" t="inlineStr">
+        <is>
+          <t>FI Name</t>
+        </is>
+      </c>
+      <c r="C2" s="7" t="inlineStr">
+        <is>
+          <t>Entity ID</t>
+        </is>
+      </c>
+      <c r="D2" s="10" t="inlineStr">
+        <is>
+          <t>Switch</t>
+        </is>
+      </c>
+      <c r="E2" s="10" t="inlineStr">
+        <is>
+          <t>Old Platform</t>
+        </is>
+      </c>
+      <c r="F2" s="10" t="inlineStr">
+        <is>
+          <t>New Platform</t>
+        </is>
+      </c>
+      <c r="G2" s="10" t="inlineStr">
+        <is>
+          <t>Service</t>
+        </is>
+      </c>
+      <c r="H2" s="10" t="inlineStr">
+        <is>
+          <t>CS Location</t>
+        </is>
+      </c>
+      <c r="I2" s="8" t="inlineStr">
+        <is>
+          <t>Total Card Count</t>
+        </is>
+      </c>
+      <c r="J2" s="8" t="inlineStr">
+        <is>
+          <t>Using OneCall IVR</t>
+        </is>
+      </c>
+      <c r="K2" s="7" t="n"/>
+      <c r="L2" s="7" t="n"/>
+      <c r="M2" s="7" t="n"/>
+      <c r="N2" s="7" t="n"/>
+      <c r="O2" s="7" t="n"/>
+      <c r="P2" s="7" t="n"/>
+      <c r="Q2" s="7" t="n"/>
+      <c r="R2" s="7" t="n"/>
+      <c r="S2" s="7" t="n"/>
+      <c r="T2" s="7" t="n"/>
+      <c r="U2" s="7" t="n"/>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A3"/>
-      <c r="B3"/>
-      <c r="C3"/>
-      <c r="D3"/>
-      <c r="E3"/>
-      <c r="F3"/>
-      <c r="G3"/>
-      <c r="H3"/>
-      <c r="I3"/>
-      <c r="J3"/>
+    <row r="3"/>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>FinanceCorp</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>ENT12345</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>FISB</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>LegacyPay</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>PaymentsOne Debit</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Basic</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Offshore</t>
+        </is>
+      </c>
+      <c r="I4" t="n">
+        <v>150000</v>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated Migration Wave to 10/22/2002
</commit_message>
<xml_diff>
--- a/Hotcard Wave Spreadsheet.xlsx
+++ b/Hotcard Wave Spreadsheet.xlsx
@@ -530,7 +530,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U4"/>
+  <dimension ref="A1:U5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
@@ -553,7 +553,7 @@
     <row r="1" ht="30" customFormat="1" customHeight="1" s="2" thickBot="1">
       <c r="A1" s="3" t="inlineStr">
         <is>
-          <t>Hotcarding Spreadsheet - Migration Wave 10/22/2001</t>
+          <t>Hotcarding Spreadsheet - Migration Wave 10/22/2002</t>
         </is>
       </c>
       <c r="B1" s="4" t="n"/>
@@ -691,6 +691,56 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2025-10-01</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>FinanceCorp</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>ENT12375</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>FISB</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>LegacyPay</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>PaymentsOne Debit</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Basic</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Offshore</t>
+        </is>
+      </c>
+      <c r="I5" t="n">
+        <v>100</v>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
Updated Migration Wave to 10/24/2002
</commit_message>
<xml_diff>
--- a/Hotcard Wave Spreadsheet.xlsx
+++ b/Hotcard Wave Spreadsheet.xlsx
@@ -530,7 +530,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U4"/>
+  <dimension ref="A1:U5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
@@ -553,7 +553,7 @@
     <row r="1" ht="30" customFormat="1" customHeight="1" s="2" thickBot="1">
       <c r="A1" s="3" t="inlineStr">
         <is>
-          <t>Hotcarding Spreadsheet - Migration Wave 10/22/2002</t>
+          <t>Hotcarding Spreadsheet - Migration Wave 10/24/2002</t>
         </is>
       </c>
       <c r="B1" s="4" t="n"/>
@@ -691,6 +691,56 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2025-11-06</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>NewFinance Ltd</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>ENT99999</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>FISN</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>OldBank</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>PaymentsNext</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Bangalore</t>
+        </is>
+      </c>
+      <c r="I5" t="n">
+        <v>500</v>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
Updated Migration Wave to 2025-10-16 00:00:00
</commit_message>
<xml_diff>
--- a/Hotcard Wave Spreadsheet.xlsx
+++ b/Hotcard Wave Spreadsheet.xlsx
@@ -530,7 +530,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U5"/>
+  <dimension ref="A1:U6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
@@ -553,7 +553,7 @@
     <row r="1" ht="30" customFormat="1" customHeight="1" s="2" thickBot="1">
       <c r="A1" s="3" t="inlineStr">
         <is>
-          <t>Hotcarding Spreadsheet - Migration Wave 10/24/2002</t>
+          <t>Hotcarding Spreadsheet - Migration Wave 2025-10-16 00:00:00</t>
         </is>
       </c>
       <c r="B1" s="4" t="n"/>
@@ -741,6 +741,58 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2025-10-16 00:00:00</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>YYY</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>123ABX007</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>FISB</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>PaymentsOne Debit</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Basic</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Offshore</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
Updated Migration Wave to Wave 10/16/2025
</commit_message>
<xml_diff>
--- a/Hotcard Wave Spreadsheet.xlsx
+++ b/Hotcard Wave Spreadsheet.xlsx
@@ -553,7 +553,7 @@
     <row r="1" ht="30" customFormat="1" customHeight="1" s="2" thickBot="1">
       <c r="A1" s="3" t="inlineStr">
         <is>
-          <t>Hotcarding Spreadsheet - Migration Wave 10/16/2025</t>
+          <t>Hotcarding Spreadsheet - Migration Wave Wave 10/16/2025</t>
         </is>
       </c>
       <c r="B1" s="4" t="n"/>
@@ -744,7 +744,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-10-16 00:00:00</t>
+          <t>10/16/2025</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">

</xml_diff>

<commit_message>
Updated Migration Wave to 2025-10-16
</commit_message>
<xml_diff>
--- a/Hotcard Wave Spreadsheet.xlsx
+++ b/Hotcard Wave Spreadsheet.xlsx
@@ -1,103 +1,60 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vivek.lade\Downloads\FIS\AAVA\Hotcard_flow\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13F7512C-4392-4341-99B8-B8B194F0E72D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="HOTCARD" sheetId="1" r:id="rId1"/>
+    <sheet name="HOTCARD" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
-  <si>
-    <t>Hotcarding Spreadsheet - Migration Wave 10/22/2001</t>
-  </si>
-  <si>
-    <t>Migration Date</t>
-  </si>
-  <si>
-    <t>FI Name</t>
-  </si>
-  <si>
-    <t>Entity ID</t>
-  </si>
-  <si>
-    <t>Switch</t>
-  </si>
-  <si>
-    <t>Old Platform</t>
-  </si>
-  <si>
-    <t>New Platform</t>
-  </si>
-  <si>
-    <t>Service</t>
-  </si>
-  <si>
-    <t>CS Location</t>
-  </si>
-  <si>
-    <t>Total Card Count</t>
-  </si>
-  <si>
-    <t>Using OneCall IVR</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="5">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Aptos"/>
       <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Aptos"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
     </font>
     <font>
-      <b/>
-      <sz val="14"/>
-      <color theme="0"/>
       <name val="Aptos"/>
       <family val="2"/>
+      <b val="1"/>
+      <color theme="0"/>
+      <sz val="14"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Aptos"/>
       <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="12"/>
     </font>
   </fonts>
   <fills count="4">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -110,7 +67,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <fgColor theme="0" tint="-0.0499893185216834"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -176,40 +133,99 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="12">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -509,94 +525,172 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="18.26953125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="30.453125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="21.26953125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.54296875" style="11" customWidth="1"/>
-    <col min="5" max="5" width="32.1796875" style="11" customWidth="1"/>
-    <col min="6" max="8" width="28.1796875" style="11" customWidth="1"/>
-    <col min="9" max="9" width="25.81640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="27.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.1796875" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.1796875" style="1"/>
+    <col width="18.26953125" customWidth="1" style="1" min="1" max="1"/>
+    <col width="30.453125" customWidth="1" style="1" min="2" max="2"/>
+    <col width="21.26953125" customWidth="1" style="1" min="3" max="3"/>
+    <col width="16.54296875" customWidth="1" style="11" min="4" max="4"/>
+    <col width="32.1796875" customWidth="1" style="11" min="5" max="5"/>
+    <col width="28.1796875" customWidth="1" style="11" min="6" max="8"/>
+    <col width="25.81640625" customWidth="1" style="1" min="9" max="9"/>
+    <col width="27.1796875" bestFit="1" customWidth="1" style="1" min="10" max="10"/>
+    <col width="9.1796875" customWidth="1" style="1" min="11" max="11"/>
+    <col width="9.1796875" customWidth="1" style="1" min="12" max="16384"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="5"/>
+    <row r="1" ht="30" customFormat="1" customHeight="1" s="2" thickBot="1">
+      <c r="A1" s="3" t="inlineStr">
+        <is>
+          <t>Hotcarding Spreadsheet - Migration Wave 2025-10-16</t>
+        </is>
+      </c>
+      <c r="B1" s="4" t="n"/>
+      <c r="C1" s="4" t="n"/>
+      <c r="D1" s="9" t="n"/>
+      <c r="E1" s="9" t="n"/>
+      <c r="F1" s="9" t="n"/>
+      <c r="G1" s="9" t="n"/>
+      <c r="H1" s="9" t="n"/>
+      <c r="I1" s="4" t="n"/>
+      <c r="J1" s="4" t="n"/>
+      <c r="K1" s="4" t="n"/>
+      <c r="L1" s="4" t="n"/>
+      <c r="M1" s="4" t="n"/>
+      <c r="N1" s="4" t="n"/>
+      <c r="O1" s="4" t="n"/>
+      <c r="P1" s="4" t="n"/>
+      <c r="Q1" s="4" t="n"/>
+      <c r="R1" s="4" t="n"/>
+      <c r="S1" s="4" t="n"/>
+      <c r="T1" s="4" t="n"/>
+      <c r="U1" s="5" t="n"/>
     </row>
-    <row r="2" spans="1:21" s="6" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
-      <c r="P2" s="7"/>
-      <c r="Q2" s="7"/>
-      <c r="R2" s="7"/>
-      <c r="S2" s="7"/>
-      <c r="T2" s="7"/>
-      <c r="U2" s="7"/>
+    <row r="2" ht="16" customFormat="1" customHeight="1" s="6">
+      <c r="A2" s="7" t="inlineStr">
+        <is>
+          <t>Migration Date</t>
+        </is>
+      </c>
+      <c r="B2" s="7" t="inlineStr">
+        <is>
+          <t>FI Name</t>
+        </is>
+      </c>
+      <c r="C2" s="7" t="inlineStr">
+        <is>
+          <t>Entity ID</t>
+        </is>
+      </c>
+      <c r="D2" s="10" t="inlineStr">
+        <is>
+          <t>Switch</t>
+        </is>
+      </c>
+      <c r="E2" s="10" t="inlineStr">
+        <is>
+          <t>Old Platform</t>
+        </is>
+      </c>
+      <c r="F2" s="10" t="inlineStr">
+        <is>
+          <t>New Platform</t>
+        </is>
+      </c>
+      <c r="G2" s="10" t="inlineStr">
+        <is>
+          <t>Service</t>
+        </is>
+      </c>
+      <c r="H2" s="10" t="inlineStr">
+        <is>
+          <t>CS Location</t>
+        </is>
+      </c>
+      <c r="I2" s="8" t="inlineStr">
+        <is>
+          <t>Total Card Count</t>
+        </is>
+      </c>
+      <c r="J2" s="8" t="inlineStr">
+        <is>
+          <t>Using OneCall IVR</t>
+        </is>
+      </c>
+      <c r="K2" s="7" t="n"/>
+      <c r="L2" s="7" t="n"/>
+      <c r="M2" s="7" t="n"/>
+      <c r="N2" s="7" t="n"/>
+      <c r="O2" s="7" t="n"/>
+      <c r="P2" s="7" t="n"/>
+      <c r="Q2" s="7" t="n"/>
+      <c r="R2" s="7" t="n"/>
+      <c r="S2" s="7" t="n"/>
+      <c r="T2" s="7" t="n"/>
+      <c r="U2" s="7" t="n"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2025-10-16</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>YYY</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>123ABX007</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>FISB</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>PaymentsOne Debit</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Basic</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Offshore</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>